<commit_message>
ng: update ng forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Nigeria/2024/mar_2024/ng_lf_tas_202403_2_participant_bay.xlsx
+++ b/LF/TAS/Nigeria/2024/mar_2024/ng_lf_tas_202403_2_participant_bay.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Nigeria\2024\mar_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F024C3E-C5A4-464A-9CAF-E835499A7D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CA8095-E907-4B8B-BB37-A0FDB589ED7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -327,10 +327,10 @@
     <t>ng_p_202403_v2</t>
   </si>
   <si>
-    <t>Select your EU</t>
-  </si>
-  <si>
-    <t>p_eu</t>
+    <t>Select your state</t>
+  </si>
+  <si>
+    <t>p_region</t>
   </si>
 </sst>
 </file>
@@ -858,7 +858,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>

</xml_diff>